<commit_message>
readying for the weekend
</commit_message>
<xml_diff>
--- a/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
+++ b/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared/data/Jack/DabTransporterPaper/currentSupDrafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{193386DA-AAA8-DF48-9656-44793ED80E2F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629BF6F0-BEAB-2C4F-AB33-91BD0735F3E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="3360" windowWidth="26840" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
+    <workbookView xWindow="50740" yWindow="3640" windowWidth="26840" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
   <si>
     <t>Reagent type (species) or resource</t>
   </si>
@@ -511,9 +511,6 @@
     <t>pFA-dabAB2</t>
   </si>
   <si>
-    <t>pFA carrying the dabA2 (Uniprot: D0KWS7) and dabB2 genes (Uniprot: D0KWS8)</t>
-  </si>
-  <si>
     <t>pET14b-dabAB2</t>
   </si>
   <si>
@@ -533,6 +530,153 @@
   </si>
   <si>
     <t>Additional information</t>
+  </si>
+  <si>
+    <r>
+      <t>Gene (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Vibrio cholera)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gene (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bacillus anthracis)</t>
+    </r>
+  </si>
+  <si>
+    <t>ncbi locus_tag: CSW01_RS07960</t>
+  </si>
+  <si>
+    <t>ncbi locus_tag: CSW01_RS07955</t>
+  </si>
+  <si>
+    <t>ncbi locus_tag: BAS2958</t>
+  </si>
+  <si>
+    <t>ncbi locus_tag: BAS2959</t>
+  </si>
+  <si>
+    <t>vcdabA</t>
+  </si>
+  <si>
+    <t>vcdabB</t>
+  </si>
+  <si>
+    <t>badabA</t>
+  </si>
+  <si>
+    <t>badabB</t>
+  </si>
+  <si>
+    <t>carrying</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>(Uniprot:</t>
+  </si>
+  <si>
+    <t>D0KWS7)</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>genes</t>
+  </si>
+  <si>
+    <t>D0KWS8)</t>
+  </si>
+  <si>
+    <t>pFA carrying the badabA2 (locus_tag: BAS2958) and badabB2 genes (locus_tag: BAS2959)</t>
+  </si>
+  <si>
+    <t>pFE-baDAB</t>
+  </si>
+  <si>
+    <t>pFE-vcDAB</t>
+  </si>
+  <si>
+    <t>pFE carrying the vcdabA2 ( locus_tag: CSW01_RS07960) and vcdabB2 genes (locus_tag: CSW01_RS07955)</t>
+  </si>
+  <si>
+    <t>pFE carrying the dabA2 (Uniprot: D0KWS7) and dabB2 genes (Uniprot: D0KWS8)</t>
+  </si>
+  <si>
+    <t>pSIM5</t>
+  </si>
+  <si>
+    <t>(Datta et al., 2006)</t>
+  </si>
+  <si>
+    <t>Heat inducible and heat curable plasmid containing lambda red recombinase</t>
+  </si>
+  <si>
+    <r>
+      <t>gDNA from</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> V. cholera</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> E7946 El Tor Ogawa was provided by Zoe Netter of the Seed laboratory at University of California, Berkeley for cloning of this gene</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">gDNA from </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>V. cholera</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> E7946 El Tor Ogawa was provided by Zoe Netter of the Seed laboratory at University of California, Berkeley for cloning of this gene</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -946,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF585AB-9C60-264A-9020-DCF94C710E80}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -975,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1114,58 +1258,64 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>40</v>
+      <c r="D12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
+      <c r="D14" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>46</v>
+      <c r="D15" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1173,195 +1323,323 @@
         <v>38</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="22" spans="1:15">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="23" spans="1:15">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" t="s">
+        <v>89</v>
+      </c>
+      <c r="L23" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" t="s">
+        <v>90</v>
+      </c>
+      <c r="N23" t="s">
+        <v>87</v>
+      </c>
+      <c r="O23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="26" spans="1:15">
+      <c r="A26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="C26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="27" spans="1:15">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="4" t="s">
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="28" spans="1:15">
+      <c r="A28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="4" t="s">
+    <row r="29" spans="1:15">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="30" spans="1:15">
+      <c r="A30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="C30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="4" t="s">
+    <row r="31" spans="1:15">
+      <c r="A31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="32" spans="1:15">
+      <c r="A32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="C32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="4" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="C33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="C35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="4" t="s">
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="C36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1371,8 +1649,8 @@
     <hyperlink ref="C9" r:id="rId3" display="https://paperpile.com/c/SilCib/M4d9" xr:uid="{8847EAED-43D8-C346-9C57-9A1A2EE81740}"/>
     <hyperlink ref="C10" r:id="rId4" display="https://paperpile.com/c/SilCib/WZ6R+PPYp" xr:uid="{651AAAFA-A4C2-E342-BCA2-4FF45890A38C}"/>
     <hyperlink ref="C11" r:id="rId5" display="https://paperpile.com/c/SilCib/q4wo" xr:uid="{09407856-D618-954D-A5FD-D4E56C24D3CD}"/>
-    <hyperlink ref="E12" r:id="rId6" display="https://paperpile.com/c/SilCib/h782" xr:uid="{46ADD60E-0D4C-E64E-B66B-7DBE9E9D6CE2}"/>
-    <hyperlink ref="E22" r:id="rId7" display="https://paperpile.com/c/SilCib/h782" xr:uid="{8515657D-3C3C-B945-93B9-F2CDA1650084}"/>
+    <hyperlink ref="E17" r:id="rId6" display="https://paperpile.com/c/SilCib/h782" xr:uid="{46ADD60E-0D4C-E64E-B66B-7DBE9E9D6CE2}"/>
+    <hyperlink ref="E29" r:id="rId7" display="https://paperpile.com/c/SilCib/h782" xr:uid="{8515657D-3C3C-B945-93B9-F2CDA1650084}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
loading current progress to move to laptop later
</commit_message>
<xml_diff>
--- a/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
+++ b/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared/data/Jack/DabTransporterPaper/currentSupDrafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629BF6F0-BEAB-2C4F-AB33-91BD0735F3E8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802BB82C-7D5B-074B-8B4C-B20CC9700DF8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50740" yWindow="3640" windowWidth="26840" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
   </bookViews>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF585AB-9C60-264A-9020-DCF94C710E80}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1653,5 +1653,6 @@
     <hyperlink ref="E29" r:id="rId7" display="https://paperpile.com/c/SilCib/h782" xr:uid="{8515657D-3C3C-B945-93B9-F2CDA1650084}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
preping for resubmission to nat micro
</commit_message>
<xml_diff>
--- a/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
+++ b/currentSupDrafts/plasmidsAndImportantReagentsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Shared/data/Jack/DabTransporterPaper/currentSupDrafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802BB82C-7D5B-074B-8B4C-B20CC9700DF8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66B6CD-A6D0-CE48-B915-F4AD34B16646}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50740" yWindow="3640" windowWidth="26840" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
+    <workbookView xWindow="50740" yWindow="3640" windowWidth="34800" windowHeight="15940" xr2:uid="{792D76EA-01C3-D54E-AC9B-27948F9F0FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>Reagent type (species) or resource</t>
   </si>
@@ -676,6 +676,30 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> E7946 El Tor Ogawa was provided by Zoe Netter of the Seed laboratory at University of California, Berkeley for cloning of this gene</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>gDNA from</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> B. anthracis Sterne</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> was provided by the Calendar and Portnoy laboratories at University of California, Berkeley for cloning of this gene</t>
     </r>
   </si>
 </sst>
@@ -1092,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF585AB-9C60-264A-9020-DCF94C710E80}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1303,6 +1327,9 @@
       <c r="D14" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="E14" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
@@ -1316,6 +1343,9 @@
       </c>
       <c r="D15" t="s">
         <v>80</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5">

</xml_diff>